<commit_message>
update delete user, import user, search multi columns
</commit_message>
<xml_diff>
--- a/datn_fe/src/components/Admin/user/data/template.xlsx
+++ b/datn_fe/src/components/Admin/user/data/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\datn\datn_fpoly\datn_fe\src\components\Admin\user\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49129997-6FE2-41DC-9669-20EBB4EF30FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58FE4B8-0893-47E2-A4F6-975AFDB644CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4008" yWindow="3360" windowWidth="19032" windowHeight="8880" xr2:uid="{E30BDF5B-668C-444F-A9EE-7373E192BEF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E30BDF5B-668C-444F-A9EE-7373E192BEF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,36 +25,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>Tên hiển thị</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Số điện thoại</t>
-  </si>
-  <si>
-    <t>kkkk</t>
-  </si>
-  <si>
-    <t>kkk2@gmail.com</t>
-  </si>
-  <si>
-    <t>kkkk5</t>
-  </si>
-  <si>
-    <t>kkkk6</t>
-  </si>
-  <si>
-    <t>kkkk7</t>
-  </si>
-  <si>
-    <t>kkk8@gmail.com</t>
-  </si>
-  <si>
-    <t>kkk9@gmail.com</t>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>test3@gmail.com</t>
+  </si>
+  <si>
+    <t>test4@gmail.com</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>last1</t>
+  </si>
+  <si>
+    <t>last2</t>
+  </si>
+  <si>
+    <t>last3</t>
+  </si>
+  <si>
+    <t>last4</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>Hochiminh</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>OTHER</t>
   </si>
 </sst>
 </file>
@@ -423,20 +468,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A817916-EDEB-41ED-8ED8-F4A4C4CB1BD5}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,58 +493,133 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>848813598</v>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2">
+        <v>12345678</v>
+      </c>
+      <c r="G2">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>848813599</v>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>12345678</v>
+      </c>
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>848813600</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>12345678</v>
+      </c>
+      <c r="G4">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>848813601</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>12345678</v>
+      </c>
+      <c r="G5">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{3AB60F06-9CD7-409A-B6C4-49EA306C333F}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{5420F77F-47D9-4289-BABB-50F1FB07E6CF}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{AE131A3B-8B45-435D-B30B-966E6F58BA9E}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{9B1A4DD2-B4BD-48DF-991B-79DEFD73FDAD}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{50F48B73-94F7-4CE4-867E-B642D187DCEC}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{526B1704-FC77-4839-9749-7F2A5923B3B0}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{57CCD430-403D-4388-9E9B-3AC70133DA2A}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{31450C30-26A7-43DA-83F6-BE8A10CFFA19}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>